<commit_message>
enter mod matrix and setup slot via shortcut
</commit_message>
<xml_diff>
--- a/src/be/NovationCircuit/midiMapping.xlsx
+++ b/src/be/NovationCircuit/midiMapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_p\midi-mplx\src\be\NovationCircuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEA483F-A7BF-4834-84D9-78AC8AA8729A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF83D46D-DE70-4B74-83E1-F7572DA389F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="664">
   <si>
     <t>section</t>
   </si>
@@ -2009,6 +2009,9 @@
   </si>
   <si>
     <t>0: Off; 1: On</t>
+  </si>
+  <si>
+    <t>modDest</t>
   </si>
 </sst>
 </file>
@@ -2859,28 +2862,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q310"/>
+  <dimension ref="A1:R310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q69" sqref="Q69"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="26.42578125" customWidth="1"/>
-    <col min="13" max="16" width="18.85546875" customWidth="1"/>
-    <col min="17" max="17" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="16" width="18.85546875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" customWidth="1"/>
+    <col min="18" max="18" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2927,10 +2932,13 @@
         <v>661</v>
       </c>
       <c r="Q1" t="s">
+        <v>663</v>
+      </c>
+      <c r="R1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2968,11 +2976,11 @@
       <c r="P2">
         <v>0</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3011,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3050,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3088,11 +3096,11 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3130,11 +3138,11 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3173,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -3211,8 +3219,11 @@
       <c r="P8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3250,8 +3261,11 @@
       <c r="P9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3290,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -3329,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -3368,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3406,8 +3420,11 @@
       <c r="P13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -3446,7 +3463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3484,11 +3501,11 @@
       <c r="P15">
         <v>0</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3527,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3565,8 +3582,11 @@
       <c r="P17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -3604,8 +3624,11 @@
       <c r="P18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3644,7 +3667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -3683,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3722,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3760,8 +3783,11 @@
       <c r="P22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3800,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -3838,8 +3864,11 @@
       <c r="P24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -3877,8 +3906,11 @@
       <c r="P25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -3916,8 +3948,11 @@
       <c r="P26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -3955,8 +3990,11 @@
       <c r="P27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -3994,11 +4032,11 @@
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -4036,11 +4074,11 @@
       <c r="P29">
         <v>0</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -4078,11 +4116,11 @@
       <c r="P30">
         <v>0</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -4120,8 +4158,11 @@
       <c r="P31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -4159,11 +4200,11 @@
       <c r="P32">
         <v>0</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -4201,11 +4242,11 @@
       <c r="P33">
         <v>0</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -4243,8 +4284,11 @@
       <c r="P34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -4283,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -4321,8 +4365,11 @@
       <c r="P36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -4361,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -4400,7 +4447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -4439,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -4478,7 +4525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>94</v>
       </c>
@@ -4516,8 +4563,11 @@
       <c r="P41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -4556,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -4595,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -4637,7 +4687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -4679,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -4720,8 +4770,11 @@
       <c r="P46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -4763,7 +4816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -4805,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -4847,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -4889,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -4931,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>94</v>
       </c>
@@ -4973,7 +5026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -5015,7 +5068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>125</v>
       </c>
@@ -5056,11 +5109,11 @@
       <c r="P54">
         <v>0</v>
       </c>
-      <c r="Q54" t="s">
+      <c r="R54" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>125</v>
       </c>
@@ -5101,11 +5154,11 @@
       <c r="P55">
         <v>0</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="R55" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>125</v>
       </c>
@@ -5147,7 +5200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>125</v>
       </c>
@@ -5189,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -5231,7 +5284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -5272,8 +5325,11 @@
       <c r="P59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>125</v>
       </c>
@@ -5315,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>125</v>
       </c>
@@ -5356,11 +5412,12 @@
       <c r="P61">
         <v>12</v>
       </c>
-      <c r="Q61" s="3" t="s">
+      <c r="Q61"/>
+      <c r="R61" s="3" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>125</v>
       </c>
@@ -5401,11 +5458,12 @@
       <c r="P62">
         <v>14</v>
       </c>
-      <c r="Q62" s="3" t="s">
+      <c r="Q62"/>
+      <c r="R62" s="3" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>125</v>
       </c>
@@ -5446,11 +5504,12 @@
       <c r="P63">
         <v>16</v>
       </c>
-      <c r="Q63" s="3" t="s">
+      <c r="Q63"/>
+      <c r="R63" s="3" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>125</v>
       </c>
@@ -5491,11 +5550,12 @@
       <c r="P64">
         <v>18</v>
       </c>
-      <c r="Q64" s="3" t="s">
+      <c r="Q64"/>
+      <c r="R64" s="3" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>125</v>
       </c>
@@ -5536,11 +5596,12 @@
       <c r="P65">
         <v>0</v>
       </c>
-      <c r="Q65" s="3" t="s">
+      <c r="Q65"/>
+      <c r="R65" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>125</v>
       </c>
@@ -5581,11 +5642,11 @@
       <c r="P66">
         <v>0</v>
       </c>
-      <c r="Q66" t="s">
+      <c r="R66" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>125</v>
       </c>
@@ -5626,11 +5687,11 @@
       <c r="P67">
         <v>0</v>
       </c>
-      <c r="Q67" t="s">
+      <c r="R67" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>125</v>
       </c>
@@ -5672,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>125</v>
       </c>
@@ -5714,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>125</v>
       </c>
@@ -5756,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>125</v>
       </c>
@@ -5797,8 +5858,11 @@
       <c r="P71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q71">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>125</v>
       </c>
@@ -5840,7 +5904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>125</v>
       </c>
@@ -5881,11 +5945,12 @@
       <c r="P73">
         <v>22</v>
       </c>
-      <c r="Q73" s="3" t="s">
+      <c r="Q73"/>
+      <c r="R73" s="3" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="74" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>125</v>
       </c>
@@ -5926,11 +5991,12 @@
       <c r="P74">
         <v>24</v>
       </c>
-      <c r="Q74" s="3" t="s">
+      <c r="Q74"/>
+      <c r="R74" s="3" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="75" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>125</v>
       </c>
@@ -5971,11 +6037,12 @@
       <c r="P75">
         <v>26</v>
       </c>
-      <c r="Q75" s="3" t="s">
+      <c r="Q75"/>
+      <c r="R75" s="3" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="76" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>125</v>
       </c>
@@ -6016,11 +6083,12 @@
       <c r="P76">
         <v>28</v>
       </c>
-      <c r="Q76" s="3" t="s">
+      <c r="Q76"/>
+      <c r="R76" s="3" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="77" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>125</v>
       </c>
@@ -6061,11 +6129,12 @@
       <c r="P77">
         <v>4</v>
       </c>
-      <c r="Q77" s="3" t="s">
+      <c r="Q77"/>
+      <c r="R77" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>169</v>
       </c>
@@ -6104,7 +6173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>169</v>
       </c>
@@ -6143,7 +6212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>169</v>
       </c>
@@ -6185,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -6227,7 +6296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>169</v>
       </c>
@@ -6269,7 +6338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>169</v>
       </c>
@@ -6311,7 +6380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>169</v>
       </c>
@@ -6353,7 +6422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>169</v>
       </c>
@@ -6395,7 +6464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>169</v>
       </c>
@@ -6436,11 +6505,11 @@
       <c r="P86">
         <v>0</v>
       </c>
-      <c r="Q86" t="s">
+      <c r="R86" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -6482,7 +6551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>169</v>
       </c>
@@ -6523,11 +6592,11 @@
       <c r="P88">
         <v>0</v>
       </c>
-      <c r="Q88" t="s">
+      <c r="R88" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>169</v>
       </c>
@@ -6569,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>169</v>
       </c>
@@ -6611,7 +6680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>169</v>
       </c>
@@ -6653,7 +6722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -6695,7 +6764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>169</v>
       </c>
@@ -6737,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>204</v>
       </c>
@@ -6775,11 +6844,11 @@
       <c r="P94">
         <v>0</v>
       </c>
-      <c r="Q94" t="s">
+      <c r="R94" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>204</v>
       </c>
@@ -6817,11 +6886,11 @@
       <c r="P95">
         <v>0</v>
       </c>
-      <c r="Q95" t="s">
+      <c r="R95" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>204</v>
       </c>
@@ -6860,7 +6929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -6898,11 +6967,11 @@
       <c r="P97">
         <v>0</v>
       </c>
-      <c r="Q97" t="s">
+      <c r="R97" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>204</v>
       </c>
@@ -6940,11 +7009,11 @@
       <c r="P98">
         <v>0</v>
       </c>
-      <c r="Q98" t="s">
+      <c r="R98" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>204</v>
       </c>
@@ -6982,11 +7051,11 @@
       <c r="P99">
         <v>0</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="R99" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>204</v>
       </c>
@@ -7025,7 +7094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>204</v>
       </c>
@@ -7063,11 +7132,11 @@
       <c r="P101">
         <v>0</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>204</v>
       </c>
@@ -7105,11 +7174,11 @@
       <c r="P102">
         <v>0</v>
       </c>
-      <c r="Q102" t="s">
+      <c r="R102" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>204</v>
       </c>
@@ -7147,11 +7216,11 @@
       <c r="P103">
         <v>0</v>
       </c>
-      <c r="Q103" t="s">
+      <c r="R103" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>204</v>
       </c>
@@ -7190,7 +7259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>204</v>
       </c>
@@ -7228,11 +7297,11 @@
       <c r="P105">
         <v>0</v>
       </c>
-      <c r="Q105" t="s">
+      <c r="R105" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>204</v>
       </c>
@@ -7270,11 +7339,11 @@
       <c r="P106">
         <v>0</v>
       </c>
-      <c r="Q106" t="s">
+      <c r="R106" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>204</v>
       </c>
@@ -7312,11 +7381,11 @@
       <c r="P107">
         <v>0</v>
       </c>
-      <c r="Q107" t="s">
+      <c r="R107" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>204</v>
       </c>
@@ -7355,7 +7424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>204</v>
       </c>
@@ -7393,11 +7462,11 @@
       <c r="P109">
         <v>0</v>
       </c>
-      <c r="Q109" t="s">
+      <c r="R109" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>204</v>
       </c>
@@ -7435,11 +7504,11 @@
       <c r="P110">
         <v>0</v>
       </c>
-      <c r="Q110" t="s">
+      <c r="R110" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>204</v>
       </c>
@@ -7477,11 +7546,11 @@
       <c r="P111">
         <v>0</v>
       </c>
-      <c r="Q111" t="s">
+      <c r="R111" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>204</v>
       </c>
@@ -7520,7 +7589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>204</v>
       </c>
@@ -7558,11 +7627,11 @@
       <c r="P113">
         <v>0</v>
       </c>
-      <c r="Q113" t="s">
+      <c r="R113" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>204</v>
       </c>
@@ -7600,11 +7669,11 @@
       <c r="P114">
         <v>0</v>
       </c>
-      <c r="Q114" t="s">
+      <c r="R114" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>204</v>
       </c>
@@ -7642,11 +7711,11 @@
       <c r="P115">
         <v>0</v>
       </c>
-      <c r="Q115" t="s">
+      <c r="R115" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>204</v>
       </c>
@@ -7685,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>204</v>
       </c>
@@ -7723,11 +7792,11 @@
       <c r="P117">
         <v>0</v>
       </c>
-      <c r="Q117" t="s">
+      <c r="R117" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>204</v>
       </c>
@@ -7765,11 +7834,11 @@
       <c r="P118">
         <v>0</v>
       </c>
-      <c r="Q118" t="s">
+      <c r="R118" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>204</v>
       </c>
@@ -7807,11 +7876,11 @@
       <c r="P119">
         <v>0</v>
       </c>
-      <c r="Q119" t="s">
+      <c r="R119" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>204</v>
       </c>
@@ -7850,7 +7919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>204</v>
       </c>
@@ -7888,11 +7957,11 @@
       <c r="P121">
         <v>0</v>
       </c>
-      <c r="Q121" t="s">
+      <c r="R121" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>204</v>
       </c>
@@ -7930,11 +7999,11 @@
       <c r="P122">
         <v>0</v>
       </c>
-      <c r="Q122" t="s">
+      <c r="R122" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>204</v>
       </c>
@@ -7972,11 +8041,11 @@
       <c r="P123">
         <v>0</v>
       </c>
-      <c r="Q123" t="s">
+      <c r="R123" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>204</v>
       </c>
@@ -8015,7 +8084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>204</v>
       </c>
@@ -8053,11 +8122,11 @@
       <c r="P125">
         <v>0</v>
       </c>
-      <c r="Q125" t="s">
+      <c r="R125" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>204</v>
       </c>
@@ -8095,11 +8164,11 @@
       <c r="P126">
         <v>0</v>
       </c>
-      <c r="Q126" t="s">
+      <c r="R126" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>204</v>
       </c>
@@ -8137,11 +8206,11 @@
       <c r="P127">
         <v>0</v>
       </c>
-      <c r="Q127" t="s">
+      <c r="R127" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>204</v>
       </c>
@@ -8180,7 +8249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>204</v>
       </c>
@@ -8218,11 +8287,11 @@
       <c r="P129">
         <v>0</v>
       </c>
-      <c r="Q129" t="s">
+      <c r="R129" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>204</v>
       </c>
@@ -8260,11 +8329,11 @@
       <c r="P130">
         <v>0</v>
       </c>
-      <c r="Q130" t="s">
+      <c r="R130" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>204</v>
       </c>
@@ -8302,11 +8371,11 @@
       <c r="P131">
         <v>0</v>
       </c>
-      <c r="Q131" t="s">
+      <c r="R131" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>204</v>
       </c>
@@ -8345,7 +8414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>204</v>
       </c>
@@ -8383,11 +8452,11 @@
       <c r="P133">
         <v>0</v>
       </c>
-      <c r="Q133" t="s">
+      <c r="R133" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>204</v>
       </c>
@@ -8425,11 +8494,11 @@
       <c r="P134">
         <v>0</v>
       </c>
-      <c r="Q134" t="s">
+      <c r="R134" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>204</v>
       </c>
@@ -8467,11 +8536,11 @@
       <c r="P135">
         <v>0</v>
       </c>
-      <c r="Q135" t="s">
+      <c r="R135" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>204</v>
       </c>
@@ -8510,7 +8579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>204</v>
       </c>
@@ -8548,11 +8617,11 @@
       <c r="P137">
         <v>0</v>
       </c>
-      <c r="Q137" t="s">
+      <c r="R137" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>204</v>
       </c>
@@ -8590,11 +8659,11 @@
       <c r="P138">
         <v>0</v>
       </c>
-      <c r="Q138" t="s">
+      <c r="R138" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>204</v>
       </c>
@@ -8632,11 +8701,11 @@
       <c r="P139">
         <v>0</v>
       </c>
-      <c r="Q139" t="s">
+      <c r="R139" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>204</v>
       </c>
@@ -8675,7 +8744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>204</v>
       </c>
@@ -8713,11 +8782,11 @@
       <c r="P141">
         <v>0</v>
       </c>
-      <c r="Q141" t="s">
+      <c r="R141" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>204</v>
       </c>
@@ -8755,11 +8824,11 @@
       <c r="P142">
         <v>0</v>
       </c>
-      <c r="Q142" t="s">
+      <c r="R142" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>204</v>
       </c>
@@ -8797,11 +8866,11 @@
       <c r="P143">
         <v>0</v>
       </c>
-      <c r="Q143" t="s">
+      <c r="R143" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>204</v>
       </c>
@@ -8840,7 +8909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>204</v>
       </c>
@@ -8878,11 +8947,11 @@
       <c r="P145">
         <v>0</v>
       </c>
-      <c r="Q145" t="s">
+      <c r="R145" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>204</v>
       </c>
@@ -8920,11 +8989,11 @@
       <c r="P146">
         <v>0</v>
       </c>
-      <c r="Q146" t="s">
+      <c r="R146" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>204</v>
       </c>
@@ -8962,11 +9031,11 @@
       <c r="P147">
         <v>0</v>
       </c>
-      <c r="Q147" t="s">
+      <c r="R147" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>204</v>
       </c>
@@ -9005,7 +9074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>204</v>
       </c>
@@ -9043,11 +9112,11 @@
       <c r="P149">
         <v>0</v>
       </c>
-      <c r="Q149" t="s">
+      <c r="R149" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>204</v>
       </c>
@@ -9085,11 +9154,11 @@
       <c r="P150">
         <v>0</v>
       </c>
-      <c r="Q150" t="s">
+      <c r="R150" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>204</v>
       </c>
@@ -9127,11 +9196,11 @@
       <c r="P151">
         <v>0</v>
       </c>
-      <c r="Q151" t="s">
+      <c r="R151" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>204</v>
       </c>
@@ -9170,7 +9239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>204</v>
       </c>
@@ -9208,11 +9277,11 @@
       <c r="P153">
         <v>0</v>
       </c>
-      <c r="Q153" t="s">
+      <c r="R153" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>204</v>
       </c>
@@ -9250,11 +9319,11 @@
       <c r="P154">
         <v>0</v>
       </c>
-      <c r="Q154" t="s">
+      <c r="R154" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>204</v>
       </c>
@@ -9292,11 +9361,11 @@
       <c r="P155">
         <v>0</v>
       </c>
-      <c r="Q155" t="s">
+      <c r="R155" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>204</v>
       </c>
@@ -9335,7 +9404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>204</v>
       </c>
@@ -9373,11 +9442,11 @@
       <c r="P157">
         <v>0</v>
       </c>
-      <c r="Q157" t="s">
+      <c r="R157" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>204</v>
       </c>
@@ -9415,11 +9484,11 @@
       <c r="P158">
         <v>0</v>
       </c>
-      <c r="Q158" t="s">
+      <c r="R158" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>204</v>
       </c>
@@ -9457,11 +9526,11 @@
       <c r="P159">
         <v>0</v>
       </c>
-      <c r="Q159" t="s">
+      <c r="R159" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>204</v>
       </c>
@@ -9500,7 +9569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>204</v>
       </c>
@@ -9538,11 +9607,11 @@
       <c r="P161">
         <v>0</v>
       </c>
-      <c r="Q161" t="s">
+      <c r="R161" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>204</v>
       </c>
@@ -9580,11 +9649,11 @@
       <c r="P162">
         <v>0</v>
       </c>
-      <c r="Q162" t="s">
+      <c r="R162" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>204</v>
       </c>
@@ -9622,11 +9691,11 @@
       <c r="P163">
         <v>0</v>
       </c>
-      <c r="Q163" t="s">
+      <c r="R163" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>204</v>
       </c>
@@ -9665,7 +9734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>204</v>
       </c>
@@ -9703,11 +9772,11 @@
       <c r="P165">
         <v>0</v>
       </c>
-      <c r="Q165" t="s">
+      <c r="R165" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>204</v>
       </c>
@@ -9745,11 +9814,11 @@
       <c r="P166">
         <v>0</v>
       </c>
-      <c r="Q166" t="s">
+      <c r="R166" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>204</v>
       </c>
@@ -9787,11 +9856,11 @@
       <c r="P167">
         <v>0</v>
       </c>
-      <c r="Q167" t="s">
+      <c r="R167" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>204</v>
       </c>
@@ -9830,7 +9899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>204</v>
       </c>
@@ -9868,11 +9937,11 @@
       <c r="P169">
         <v>0</v>
       </c>
-      <c r="Q169" t="s">
+      <c r="R169" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>204</v>
       </c>
@@ -9910,11 +9979,11 @@
       <c r="P170">
         <v>0</v>
       </c>
-      <c r="Q170" t="s">
+      <c r="R170" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>204</v>
       </c>
@@ -9952,11 +10021,11 @@
       <c r="P171">
         <v>0</v>
       </c>
-      <c r="Q171" t="s">
+      <c r="R171" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>204</v>
       </c>
@@ -9995,7 +10064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>204</v>
       </c>
@@ -10033,11 +10102,11 @@
       <c r="P173">
         <v>0</v>
       </c>
-      <c r="Q173" t="s">
+      <c r="R173" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>367</v>
       </c>
@@ -10073,7 +10142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>367</v>
       </c>
@@ -10112,7 +10181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>367</v>
       </c>

</xml_diff>

<commit_message>
led mapping on lcxl (needs debugging)
</commit_message>
<xml_diff>
--- a/src/be/NovationCircuit/midiMapping.xlsx
+++ b/src/be/NovationCircuit/midiMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_p\midi-mplx\src\be\NovationCircuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF83D46D-DE70-4B74-83E1-F7572DA389F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D388A1C4-1755-40A7-A8F8-FD95CDF552F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5145" yWindow="1275" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="midiMapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="671">
   <si>
     <t>section</t>
   </si>
@@ -2012,6 +2012,27 @@
   </si>
   <si>
     <t>modDest</t>
+  </si>
+  <si>
+    <t>simpleColor</t>
+  </si>
+  <si>
+    <t>greenH</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>amberH</t>
+  </si>
+  <si>
+    <t>redL</t>
+  </si>
+  <si>
+    <t>redH</t>
+  </si>
+  <si>
+    <t>greenL</t>
   </si>
 </sst>
 </file>
@@ -2862,10 +2883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R310"/>
+  <dimension ref="A1:S310"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y87" sqref="Y87:Z87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,14 +2899,14 @@
     <col min="8" max="8" width="12.28515625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="26.42578125" hidden="1" customWidth="1"/>
-    <col min="13" max="16" width="18.85546875" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" customWidth="1"/>
-    <col min="18" max="18" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="17" width="18.85546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="255.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2937,8 +2958,11 @@
       <c r="R1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2979,8 +3003,11 @@
       <c r="R2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3018,8 +3045,11 @@
       <c r="P3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3057,8 +3087,11 @@
       <c r="P4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3099,8 +3132,11 @@
       <c r="R5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3141,8 +3177,11 @@
       <c r="R6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3180,8 +3219,11 @@
       <c r="P7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -3222,8 +3264,11 @@
       <c r="Q8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3264,8 +3309,11 @@
       <c r="Q9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3303,8 +3351,11 @@
       <c r="P10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -3342,8 +3393,11 @@
       <c r="P11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -3381,8 +3435,11 @@
       <c r="P12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3423,8 +3480,11 @@
       <c r="Q13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -3462,8 +3522,11 @@
       <c r="P14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3504,8 +3567,11 @@
       <c r="R15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3543,8 +3609,11 @@
       <c r="P16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3585,8 +3654,11 @@
       <c r="Q17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -3627,8 +3699,11 @@
       <c r="Q18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3666,8 +3741,11 @@
       <c r="P19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -3705,8 +3783,11 @@
       <c r="P20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3744,8 +3825,11 @@
       <c r="P21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3786,8 +3870,11 @@
       <c r="Q22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3825,8 +3912,11 @@
       <c r="P23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -3867,8 +3957,11 @@
       <c r="Q24">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -3909,8 +4002,11 @@
       <c r="Q25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -3951,8 +4047,11 @@
       <c r="Q26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -3993,8 +4092,11 @@
       <c r="Q27">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -4035,8 +4137,11 @@
       <c r="R28" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -4077,8 +4182,11 @@
       <c r="R29" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -4119,8 +4227,11 @@
       <c r="R30" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -4161,8 +4272,11 @@
       <c r="Q31">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -4203,8 +4317,11 @@
       <c r="R32" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -4245,8 +4362,11 @@
       <c r="R33" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -4287,8 +4407,11 @@
       <c r="Q34">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -4326,8 +4449,11 @@
       <c r="P35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -4368,8 +4494,11 @@
       <c r="Q36">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -4407,8 +4536,11 @@
       <c r="P37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -4446,8 +4578,11 @@
       <c r="P38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -4485,8 +4620,11 @@
       <c r="P39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -4524,8 +4662,11 @@
       <c r="P40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>94</v>
       </c>
@@ -4566,8 +4707,11 @@
       <c r="Q41">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -4605,8 +4749,11 @@
       <c r="P42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -4644,8 +4791,11 @@
       <c r="P43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S43" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -4686,8 +4836,11 @@
       <c r="P44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S44" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -4728,8 +4881,11 @@
       <c r="P45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S45" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -4773,8 +4929,11 @@
       <c r="Q46">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S46" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -4815,8 +4974,11 @@
       <c r="P47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S47" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -4857,8 +5019,11 @@
       <c r="P48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S48" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -4899,8 +5064,11 @@
       <c r="P49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S49" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -4941,8 +5109,11 @@
       <c r="P50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S50" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -4983,8 +5154,11 @@
       <c r="P51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S51" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>94</v>
       </c>
@@ -5025,8 +5199,11 @@
       <c r="P52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S52" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -5067,8 +5244,11 @@
       <c r="P53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S53" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>125</v>
       </c>
@@ -5112,8 +5292,11 @@
       <c r="R54" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S54" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>125</v>
       </c>
@@ -5157,8 +5340,11 @@
       <c r="R55" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S55" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>125</v>
       </c>
@@ -5199,8 +5385,11 @@
       <c r="P56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S56" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>125</v>
       </c>
@@ -5241,8 +5430,11 @@
       <c r="P57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S57" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -5283,8 +5475,11 @@
       <c r="P58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S58" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -5328,8 +5523,11 @@
       <c r="Q59">
         <v>14</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S59" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>125</v>
       </c>
@@ -5370,8 +5568,11 @@
       <c r="P60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S60" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>125</v>
       </c>
@@ -5416,8 +5617,11 @@
       <c r="R61" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S61" s="3" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>125</v>
       </c>
@@ -5462,8 +5666,11 @@
       <c r="R62" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S62" s="3" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>125</v>
       </c>
@@ -5508,8 +5715,11 @@
       <c r="R63" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S63" s="3" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>125</v>
       </c>
@@ -5554,8 +5764,11 @@
       <c r="R64" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S64" s="3" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>125</v>
       </c>
@@ -5600,8 +5813,11 @@
       <c r="R65" s="3" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S65" s="3" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>125</v>
       </c>
@@ -5645,8 +5861,11 @@
       <c r="R66" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S66" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>125</v>
       </c>
@@ -5690,8 +5909,11 @@
       <c r="R67" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S67" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>125</v>
       </c>
@@ -5732,8 +5954,11 @@
       <c r="P68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S68" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>125</v>
       </c>
@@ -5774,8 +5999,11 @@
       <c r="P69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S69" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>125</v>
       </c>
@@ -5816,8 +6044,11 @@
       <c r="P70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S70" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>125</v>
       </c>
@@ -5861,8 +6092,11 @@
       <c r="Q71">
         <v>15</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S71" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>125</v>
       </c>
@@ -5903,8 +6137,11 @@
       <c r="P72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S72" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>125</v>
       </c>
@@ -5949,8 +6186,11 @@
       <c r="R73" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S73" s="3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>125</v>
       </c>
@@ -5995,8 +6235,11 @@
       <c r="R74" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S74" s="3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>125</v>
       </c>
@@ -6041,8 +6284,11 @@
       <c r="R75" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S75" s="3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>125</v>
       </c>
@@ -6087,8 +6333,11 @@
       <c r="R76" s="3" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S76" s="3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>125</v>
       </c>
@@ -6133,8 +6382,11 @@
       <c r="R77" s="3" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S77" s="3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>169</v>
       </c>
@@ -6172,8 +6424,11 @@
       <c r="P78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S78" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>169</v>
       </c>
@@ -6211,8 +6466,11 @@
       <c r="P79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S79" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>169</v>
       </c>
@@ -6253,8 +6511,11 @@
       <c r="P80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S80" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -6295,8 +6556,11 @@
       <c r="P81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S81" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>169</v>
       </c>
@@ -6337,8 +6601,11 @@
       <c r="P82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S82" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>169</v>
       </c>
@@ -6379,8 +6646,11 @@
       <c r="P83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S83" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>169</v>
       </c>
@@ -6421,8 +6691,11 @@
       <c r="P84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S84" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>169</v>
       </c>
@@ -6463,8 +6736,11 @@
       <c r="P85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S85" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>169</v>
       </c>
@@ -6508,8 +6784,11 @@
       <c r="R86" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S86" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -6550,8 +6829,11 @@
       <c r="P87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S87" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>169</v>
       </c>
@@ -6595,8 +6877,11 @@
       <c r="R88" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S88" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>169</v>
       </c>
@@ -6637,8 +6922,11 @@
       <c r="P89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S89" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>169</v>
       </c>
@@ -6679,8 +6967,11 @@
       <c r="P90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S90" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>169</v>
       </c>
@@ -6721,8 +7012,11 @@
       <c r="P91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S91" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -6763,8 +7057,11 @@
       <c r="P92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S92" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>169</v>
       </c>
@@ -6805,8 +7102,11 @@
       <c r="P93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S93" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>204</v>
       </c>
@@ -6848,7 +7148,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>204</v>
       </c>
@@ -6890,7 +7190,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>204</v>
       </c>

</xml_diff>